<commit_message>
# Conclusions 47 - 4 layers - ('relu', 'relu') with batch [350,400,450] and widths [350,400,450] - Best test accuracy: 400 batch, 450 width: test accuracy 0.9848 - 2nd best: 350 batch, 400 width: test accuracy 0.9845 - 3rd best: 450 batch, 450 width ### Conclusions going forward: - Try batch 400, 450 with width 500
</commit_message>
<xml_diff>
--- a/output/46_5_layers_relu_tanh_sigmoid_300_300/full.xlsx
+++ b/output/46_5_layers_relu_tanh_sigmoid_300_300/full.xlsx
@@ -1,37 +1,110 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkrichev\Documents\Yoni\DataScience\data-science-ml-dl-mnist\output\46_5_layers_relu_tanh_sigmoid_300_300\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+  <si>
+    <t>Validate loss improvement delta</t>
+  </si>
+  <si>
+    <t>Validate loss improvement patience</t>
+  </si>
+  <si>
+    <t>Restore best weights</t>
+  </si>
+  <si>
+    <t>Max num epochs</t>
+  </si>
+  <si>
+    <t>Batch size</t>
+  </si>
+  <si>
+    <t>Num layers</t>
+  </si>
+  <si>
+    <t>Hidden funcs</t>
+  </si>
+  <si>
+    <t>Hidden width</t>
+  </si>
+  <si>
+    <t>Learning rate</t>
+  </si>
+  <si>
+    <t>Shuffle seed</t>
+  </si>
+  <si>
+    <t>Test Accuracy</t>
+  </si>
+  <si>
+    <t>Test Loss</t>
+  </si>
+  <si>
+    <t>Train Time</t>
+  </si>
+  <si>
+    <t>Loss * Time</t>
+  </si>
+  <si>
+    <t>Validate Accuracy</t>
+  </si>
+  <si>
+    <t>Train Accuracy</t>
+  </si>
+  <si>
+    <t>Validate Loss</t>
+  </si>
+  <si>
+    <t>Train Loss</t>
+  </si>
+  <si>
+    <t>Num epochs</t>
+  </si>
+  <si>
+    <t>Average epoch time</t>
+  </si>
+  <si>
+    <t>('relu', 'tanh', 'sigmoid')</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,26 +119,49 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,323 +449,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Validate loss improvement delta</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Validate loss improvement patience</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Restore best weights</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Max num epochs</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Batch size</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Num layers</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Hidden funcs</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Hidden width</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Learning rate</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Shuffle seed</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Test Accuracy</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Test Loss</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Train Time</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Loss * Time</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Validate Accuracy</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Train Accuracy</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Validate Loss</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Train Loss</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Num epochs</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Average epoch time</t>
-        </is>
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>1E-4</v>
+      </c>
+      <c r="C2">
         <v>10</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>1000</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>300</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>('relu', 'tanh', 'sigmoid')</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2">
         <v>300</v>
       </c>
-      <c r="J2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="J2">
+        <v>1E-3</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="L2" t="n">
-        <v>0.9822999835014343</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.0684</v>
-      </c>
-      <c r="N2" t="n">
-        <v>204.906</v>
-      </c>
-      <c r="O2" t="n">
-        <v>14.0156</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.9998000264167786</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.9997000098228455</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0.0011</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.0013</v>
-      </c>
-      <c r="T2" t="n">
+      <c r="L2">
+        <v>0.98229998350143433</v>
+      </c>
+      <c r="M2">
+        <v>6.8400000000000002E-2</v>
+      </c>
+      <c r="N2">
+        <v>204.90600000000001</v>
+      </c>
+      <c r="O2">
+        <v>14.015599999999999</v>
+      </c>
+      <c r="P2">
+        <v>0.99980002641677856</v>
+      </c>
+      <c r="Q2">
+        <v>0.99970000982284546</v>
+      </c>
+      <c r="R2">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="S2">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="T2">
         <v>27</v>
       </c>
-      <c r="U2" t="n">
-        <v>7.5891</v>
+      <c r="U2">
+        <v>7.5891000000000002</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3">
+        <v>1E-4</v>
+      </c>
+      <c r="C3">
         <v>10</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>1000</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>300</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>('relu', 'tanh', 'sigmoid')</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
         <v>300</v>
       </c>
-      <c r="J3" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="K3" t="n">
+      <c r="J3">
+        <v>1E-3</v>
+      </c>
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="L3" t="n">
-        <v>0.9854000210762024</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.07149999999999999</v>
-      </c>
-      <c r="N3" t="n">
-        <v>292.881</v>
-      </c>
-      <c r="O3" t="n">
-        <v>20.941</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.9994999766349792</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.9988999962806702</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.0017</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0.0033</v>
-      </c>
-      <c r="T3" t="n">
+      <c r="L3">
+        <v>0.98540002107620239</v>
+      </c>
+      <c r="M3">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="N3">
+        <v>292.88099999999997</v>
+      </c>
+      <c r="O3">
+        <v>20.940999999999999</v>
+      </c>
+      <c r="P3">
+        <v>0.99949997663497925</v>
+      </c>
+      <c r="Q3">
+        <v>0.99889999628067017</v>
+      </c>
+      <c r="R3">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="S3">
+        <v>3.3E-3</v>
+      </c>
+      <c r="T3">
         <v>34</v>
       </c>
-      <c r="U3" t="n">
-        <v>8.614100000000001</v>
+      <c r="U3">
+        <v>8.6141000000000005</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4">
+        <v>1E-4</v>
+      </c>
+      <c r="C4">
         <v>10</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>1000</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>300</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>5</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>('relu', 'tanh', 'sigmoid')</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4">
         <v>300</v>
       </c>
-      <c r="J4" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="J4">
+        <v>1E-3</v>
+      </c>
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="L4" t="n">
-        <v>0.9828000068664551</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.0713</v>
-      </c>
-      <c r="N4" t="n">
-        <v>296.205</v>
-      </c>
-      <c r="O4" t="n">
-        <v>21.1194</v>
-      </c>
-      <c r="P4" t="n">
+      <c r="L4">
+        <v>0.98280000686645508</v>
+      </c>
+      <c r="M4">
+        <v>7.1300000000000002E-2</v>
+      </c>
+      <c r="N4">
+        <v>296.20499999999998</v>
+      </c>
+      <c r="O4">
+        <v>21.119399999999999</v>
+      </c>
+      <c r="P4">
         <v>1</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q4">
         <v>1</v>
       </c>
-      <c r="R4" t="n">
+      <c r="R4">
         <v>0</v>
       </c>
-      <c r="S4" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="T4" t="n">
+      <c r="S4">
+        <v>1E-4</v>
+      </c>
+      <c r="T4">
         <v>32</v>
       </c>
-      <c r="U4" t="n">
-        <v>9.256399999999999</v>
+      <c r="U4">
+        <v>9.2563999999999993</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>